<commit_message>
Finalizado a parte de metodologia
</commit_message>
<xml_diff>
--- a/xls/campos_formulario.xlsx
+++ b/xls/campos_formulario.xlsx
@@ -14,10 +14,139 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Atributo</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Identificador do Estudo</t>
+  </si>
+  <si>
+    <t>ID único para cada estudo, por exemplo IE01</t>
+  </si>
+  <si>
+    <t>Data de Extração</t>
+  </si>
+  <si>
+    <t>Data no qual a extração foi conduzida (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Nome do Extrator</t>
+  </si>
+  <si>
+    <t>Nome da pessoa responsável pela extração</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Autor do estudo</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Ano de publicação do estudo</t>
+  </si>
+  <si>
+    <t>Título</t>
+  </si>
+  <si>
+    <t>Título do Estudo</t>
+  </si>
+  <si>
+    <t>Tipo de Publicação</t>
+  </si>
+  <si>
+    <t>Artigo de journal ou conferência, dissertação, tese ou whitepaper</t>
+  </si>
+  <si>
+    <t>Objetivo do Estudo</t>
+  </si>
+  <si>
+    <t>Quais foram os objetivos do estudo?</t>
+  </si>
+  <si>
+    <t>Metodologia do Estudo</t>
+  </si>
+  <si>
+    <t>Quais foram as metodologias utilizadas no estudo?</t>
+  </si>
+  <si>
+    <t>Descobertas e Resultados</t>
+  </si>
+  <si>
+    <t>Quais foram os resultados e descobertas do estudo</t>
+  </si>
+  <si>
+    <t>Nome da Ferramenta</t>
+  </si>
+  <si>
+    <t>Nome da ferramenta</t>
+  </si>
+  <si>
+    <t>Desenvolvedor</t>
+  </si>
+  <si>
+    <t>Pessoa ou empresa responsável pelo desenvolvimento</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Site da internet da ferramenta</t>
+  </si>
+  <si>
+    <t>Objetivo da Ferramenta</t>
+  </si>
+  <si>
+    <t>Qual funcionalidade principal da ferramenta</t>
+  </si>
+  <si>
+    <t>Tipo de Arquitetura da Ferramenta</t>
+  </si>
+  <si>
+    <t>Cliente/Servidor ou Web ou desktop</t>
+  </si>
+  <si>
+    <t>Tipo de Licença da Ferramenta</t>
+  </si>
+  <si>
+    <t>Software livre ou proprietário</t>
+  </si>
+  <si>
+    <t>Avaliação da Ferramenta</t>
+  </si>
+  <si>
+    <t>Como a ferramenta foi avaliada</t>
+  </si>
+  <si>
+    <t>Estudo de Casos</t>
+  </si>
+  <si>
+    <t>Existe algum estudo de caso ou aplicação real da ferramenta</t>
+  </si>
+  <si>
+    <t>Ramo de Atuação</t>
+  </si>
+  <si>
+    <t>Qual setor da economia (governos, medicina, setor financeiro) a ferramenta já foi utilizada?</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -83,9 +212,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -106,17 +243,241 @@
     <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>